<commit_message>
feat: add antibiotic fields
</commit_message>
<xml_diff>
--- a/tests/mock_excel_db/plasmids.xlsx
+++ b/tests/mock_excel_db/plasmids.xlsx
@@ -25,9 +25,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
     <t xml:space="preserve">Resistance</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Antibiotics</t>
   </si>
   <si>
     <t xml:space="preserve">Origin</t>
@@ -37,6 +40,9 @@
   </si>
   <si>
     <t xml:space="preserve">p15A</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Amp,Kan</t>
   </si>
 </sst>
 </file>
@@ -133,23 +139,22 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:B3"/>
+  <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="bottomLeft" activeCell="E24" activeCellId="0" sqref="E24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.54296875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="15.37"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="14.02"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="22.47"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="22.86"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="18.82"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="15.95"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1024" min="1024" style="0" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="2" style="0" width="14.02"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="22.47"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="22.86"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="18.82"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="15.95"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -159,13 +164,21 @@
       <c r="B1" s="0" t="s">
         <v>1</v>
       </c>
+      <c r="C1" s="0" t="s">
+        <v>2</v>
+      </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
-      <c r="B3" s="0" t="s">
-        <v>3</v>
+      <c r="C3" s="0" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B4" s="0" t="s">
+        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>